<commit_message>
ajout fichier optimisation draft
</commit_message>
<xml_diff>
--- a/Analyse/audit.xlsx
+++ b/Analyse/audit.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="205">
   <si>
     <t>Vérification des critères d'Accessibilité</t>
   </si>
@@ -592,7 +592,7 @@
     <t>utilisation de mot clé de localistion incorrecte (Paris au lieu de Lyon)</t>
   </si>
   <si>
-    <t>N°</t>
+    <t>Thème</t>
   </si>
   <si>
     <t>Catégorie</t>
@@ -616,6 +616,9 @@
     <t>Actions réalisée</t>
   </si>
   <si>
+    <t>n°</t>
+  </si>
+  <si>
     <t>Amélioration de l'accessibilité</t>
   </si>
   <si>
@@ -643,7 +646,7 @@
     <t>Ajouter une autre mise en forme en plus de la couleur sur les liens et s'assurer qu'ils sont bien focusables</t>
   </si>
   <si>
-    <t>ajout d'une bordure au survol du lien</t>
+    <t>ajout d'une bordure au survol sur les liens de navigtion</t>
   </si>
   <si>
     <t>Détection de mots clés de très petite taille avec une police de la même couleur que le fond</t>
@@ -710,7 +713,7 @@
     </r>
   </si>
   <si>
-    <t>supprimer ces mots clés.Utiliser plutôt les mots clés dans le contenu de la page (titre, paragraphe ect)</t>
+    <t>Supprimer les mots clés masqués.Utiliser plutôt les mots clés dans le contenu de la page (titre, paragraphe ect)</t>
   </si>
   <si>
     <t>Contenu des attibuts alt non pertinents</t>
@@ -719,28 +722,37 @@
     <t>L'objectif des attributs alt servent à décrire l'image et non à y insérer une liste de mots clés qui n'ont pas de rapport avec l'image présenté</t>
   </si>
   <si>
-    <t>Mettre à jour les balises alt de toutes les images pour les décrire, si possible, avec des mots clés</t>
-  </si>
-  <si>
-    <t>x</t>
+    <t>Mettre à jour les balises alt pour donner une description pertinente aux images</t>
   </si>
   <si>
     <t>Les citations contenus dans la page web sont sous forme d'image de texte</t>
   </si>
   <si>
-    <t>Les images sous forme de texte ne seront pas accessible à tous à moins d'y ajouter le texte brut en étiquette. Ces images créeent également erreur de responsive en dessous de 600 px</t>
+    <t>Les images sous forme de texte ne seront pas accessible à tous à moins d'y ajouter le texte brut en étiquette. Ces images créeent également erreur de responsive</t>
   </si>
   <si>
     <t>remplacer les textes sous forme d'image par des textes "brut"</t>
   </si>
   <si>
+    <t xml:space="preserve">SEO ON-PAGE </t>
+  </si>
+  <si>
+    <t>balise &lt;title&gt; et &lt;description&gt; ne sont pas complétées</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les balises &lt;title&gt; et description sont importantes en SEO car elles sont utilisées par google pour décrire le contenu de la page </t>
+  </si>
+  <si>
+    <t>Renseigner les informations sur le titre et la description de la page en utilisant des mots clés</t>
+  </si>
+  <si>
     <t>L'attribut "lang" n'est pas renseigné</t>
   </si>
   <si>
     <t>Dans le header, la balise "html lang" a pour valeur "Default", ce qui n'est pas une propriété valable</t>
   </si>
   <si>
-    <t xml:space="preserve">Afin de mieux localiser le site, toujours indique la langue </t>
+    <t xml:space="preserve">Afin de mieux localiser le site, toujours indiquer la langue </t>
   </si>
   <si>
     <t>ajout de l'attibut lang="fr"</t>
@@ -752,65 +764,67 @@
     <t>Amélioration de la vitesse du site</t>
   </si>
   <si>
-    <t xml:space="preserve">SEO ON-PAGE </t>
-  </si>
-  <si>
     <t>La taille des images n'est pas adaptée au conteneur</t>
   </si>
   <si>
     <t>Impacte sur la taille du site et  sa vitesse de chargement. Une mauvaise experience utilisateur va avoir des consequence sur le SEO</t>
   </si>
   <si>
-    <t>optimiser la taille des images en fonction de leur contenant</t>
-  </si>
-  <si>
-    <t>redimention des image avec</t>
+    <t>Optimiser la taille des images en fonction de leur contenant</t>
+  </si>
+  <si>
+    <t>redimention des images du portofolio à 270 px</t>
   </si>
   <si>
     <t>Les images ne sont pas compressées</t>
   </si>
   <si>
-    <t>1 - eviter les redirection et contenus inutiles 
-2 - avoir des pages légères
-4- éviter le contenu dupliqué</t>
-  </si>
-  <si>
-    <t>compresser les images avec imagify.io</t>
-  </si>
-  <si>
-    <t>les pages ne sont pas compressées</t>
-  </si>
-  <si>
-    <t>1 - eviter les redirection et contenus inutiles 
-2 - avoir des pages légères
-5- éviter le contenu dupliqué</t>
-  </si>
-  <si>
-    <t>compresser les pages web et css avec Gzip et créer un fichier .htaccess</t>
+    <t>Impacte sur la taille du site et  sa vitesse de chargement. Une mauvaise experience utilisateur va avoir des conséquences sur le SEO</t>
+  </si>
+  <si>
+    <t>Toujours compresser les images afin d'alléger leur poids</t>
+  </si>
+  <si>
+    <t>compresser les images, optimiser les formats des images (ex: logo en svg)</t>
   </si>
   <si>
     <t>Les codes de sont pas minifier</t>
   </si>
   <si>
-    <t>minifier le code html, css et javascript</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minifier le code html, css et javascript avec </t>
-  </si>
-  <si>
-    <t>vitesse et taille du site</t>
-  </si>
-  <si>
-    <t>cela va impacter la taille du site et donc sa vitesse de chargement</t>
-  </si>
-  <si>
-    <t>mettre en cache navigateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">débloquer le téléchargement de la page </t>
-  </si>
-  <si>
-    <t>version mobile responsive</t>
+    <t>Minifier le code html, css et javascript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minifier le code html, css et javascript </t>
+  </si>
+  <si>
+    <t>Les attributs defer ou async ne sont pas définis</t>
+  </si>
+  <si>
+    <t>Javascrip est utilisé pour l'esthétic du site et n'a donc pas besoin d'être chargé en même temps que le chargement de la page</t>
+  </si>
+  <si>
+    <t>Retarder le lancement des scripts js avec l'attribut "defer" permet de gagnaer en vitesse de chargement de la page</t>
+  </si>
+  <si>
+    <t>Ajouter l'attribut "defer" aux balises script</t>
+  </si>
+  <si>
+    <t>La politique de cache n'est pas efficace</t>
+  </si>
+  <si>
+    <t>La politique de cache est paramétrée sur 10min</t>
+  </si>
+  <si>
+    <t>Pour  un chargement plus rapide, il faut une politique de mise en cache navigateur efficace</t>
+  </si>
+  <si>
+    <t>paramétrer le mise en cache via le fichier .htaccess (ex:1 mois de mise en cache sur les images)</t>
+  </si>
+  <si>
+    <t>pas possible de modifier la politique mise en de cache sur github pages (10min par défaut)</t>
+  </si>
+  <si>
+    <t>version mobile non responsive</t>
   </si>
   <si>
     <t>Des bugs sont identifiés sur la version mobile responsive (texte coupé...)</t>
@@ -819,23 +833,33 @@
     <t>corriger les bugs de la version mobile responsive</t>
   </si>
   <si>
-    <t xml:space="preserve">structure technique </t>
-  </si>
-  <si>
-    <t xml:space="preserve">titres, images, contenus non complets et mal ordonnés </t>
-  </si>
-  <si>
-    <t>avoir un menu claire et simple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 - ajout des balises meta robot, 
-2- renseigner les balises meta title et description
-3 - ajout d'une balise canonique sur la page pirincipale 
-4 - correction des titres et de leur ordre d'apparition: un seul H1, suivi de plusieurs h2 puis suivi de H3 
-5 - Les mots-clés doivent apparaître dans les balises de titres, les paragraphes et les attributs
+    <t>Absence de balise méta "robot"</t>
+  </si>
+  <si>
+    <t>La balise meta robots permet d'indiquer au moteur s'il doit ou non indexer un contenu, ou s'il  doit  ou non suivre les liens qu’il rencontre dans ce contenu. En l'absence de cette balise, la page risque de ne pas être indéxée</t>
+  </si>
+  <si>
+    <t>Toujours renseigner la balaise meta robots avec les attributs "follow" ou "not follow"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout de balises meta robots "follow" dans la partie "head" 
 </t>
   </si>
   <si>
+    <t>Problème identifié dans la structure hierarchique du code Html</t>
+  </si>
+  <si>
+    <t>Le code est mal structuré( h3 avant h2), il utilise peu de balises sémantiques. Si le code est mal structurer, le navigateur pourrait cesser d'indexer le contenu de la page</t>
+  </si>
+  <si>
+    <t>Toujours utiliser des balises semantiques et respecter d'ordre hierarchique des titres dans le code (un seul h1 suivis de h2 puis de h3...)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Correction des titres et de leur ordre d'apparition: un seul H1, suivi de plusieurs h2 puis suivi de H3 
+</t>
+  </si>
+  <si>
     <t>liens depuis la page</t>
   </si>
   <si>
@@ -843,16 +867,37 @@
   </si>
   <si>
     <t>un nombre de liens trop nombreux peut être assimilé à du spam
-diversifier les ancres, ajouter l'attribut rel="follow" ou rel="not follow"</t>
+ajouter des ancres, ajouter l'attribut rel="follow" ou rel="not follow"</t>
   </si>
   <si>
     <t>Retirer les liens non pertinent (annuaires..)</t>
   </si>
   <si>
+    <t>Amélioration du contenu</t>
+  </si>
+  <si>
+    <t>pas de mot clé dans le titre H1</t>
+  </si>
+  <si>
+    <t>Les mots-clés doivent apparaître dans les balises de titres, les paragraphes et les attributs</t>
+  </si>
+  <si>
     <t>mots clés et contenu</t>
   </si>
   <si>
     <t>Ajout de machine à contenu permettant de créer une image d'expert en utilisant des mots clés (ex: articles spécialisés, actualités, politique de recrutement de l'entreprise)</t>
+  </si>
+  <si>
+    <t>pas de mise à jour régulière du seo</t>
+  </si>
+  <si>
+    <t>faire un suivi trimestiel de l'évolution du seo</t>
+  </si>
+  <si>
+    <t>1 - utilisation de google analitics et google search console</t>
+  </si>
+  <si>
+    <t>seo off page</t>
   </si>
   <si>
     <t>pas de composant locale dans la stratégie SEO</t>
@@ -881,18 +926,6 @@
     <t>se faire connaitre et encourager les avis positifs</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>pas de mise à jour régulière du seo</t>
-  </si>
-  <si>
-    <t>faire un suivi trimestiel de l'évolution du seo</t>
-  </si>
-  <si>
-    <t>1 - utilisation de google analitics et google search console</t>
-  </si>
-  <si>
     <t>mots clés généraux</t>
   </si>
   <si>
@@ -900,6 +933,9 @@
   </si>
   <si>
     <t>agence de web design</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
   <si>
     <t>agence internet</t>
@@ -970,10 +1006,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="36">
     <font>
@@ -1017,13 +1053,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -1046,6 +1075,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1107,24 +1143,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1145,16 +1166,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1165,36 +1179,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1213,8 +1197,60 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1234,18 +1270,12 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1255,7 +1285,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.4"/>
+        <fgColor theme="9" tint="-0.25"/>
+        <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.25"/>
+        <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.25"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.25"/>
         <bgColor rgb="FF7030A0"/>
       </patternFill>
     </fill>
@@ -1291,139 +1345,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1433,32 +1511,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1470,9 +1524,7 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -1495,16 +1547,58 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1538,32 +1632,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1597,18 +1670,39 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1626,134 +1720,134 @@
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="37" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1761,16 +1855,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1778,91 +1874,98 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2138,216 +2241,216 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="106.333333333333" style="35" customWidth="1"/>
-    <col min="2" max="2" width="28.1111111111111" style="35" customWidth="1"/>
-    <col min="3" max="3" width="25.7777777777778" style="35" customWidth="1"/>
+    <col min="1" max="1" width="106.333333333333" style="37" customWidth="1"/>
+    <col min="2" max="2" width="28.1111111111111" style="37" customWidth="1"/>
+    <col min="3" max="3" width="25.7777777777778" style="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="62" customHeight="1" spans="1:8">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-    </row>
-    <row r="2" s="35" customFormat="1" ht="18" spans="1:3">
-      <c r="A2" s="39" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+    </row>
+    <row r="2" s="37" customFormat="1" ht="18" spans="1:3">
+      <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="18" spans="1:3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
     </row>
     <row r="4" ht="30" spans="1:3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="43" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="45" spans="1:3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="44" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" ht="18" spans="1:3">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
     </row>
     <row r="7" ht="31.5" spans="1:3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="43" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="43"/>
     </row>
     <row r="9" ht="18" spans="1:3">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
     </row>
     <row r="10" ht="45" spans="1:3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="43" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:3">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="43"/>
     </row>
     <row r="12" ht="18" spans="1:3">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
     </row>
     <row r="13" ht="30.75" spans="1:3">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="43" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" ht="30" spans="1:3">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="43" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" ht="30" spans="1:3">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="43"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="43"/>
     </row>
     <row r="17" ht="18" spans="1:3">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
     </row>
     <row r="18" ht="45" spans="1:3">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="15"/>
+      <c r="C18" s="43"/>
     </row>
     <row r="19" ht="18" spans="1:3">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
     </row>
     <row r="20" ht="30" spans="1:3">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="15"/>
+      <c r="C20" s="43"/>
     </row>
     <row r="21" ht="18" spans="1:3">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
     </row>
     <row r="22" ht="15.75" spans="1:3">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="43" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="23" ht="45" spans="1:3">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="47" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="13" t="s">
@@ -2358,7 +2461,7 @@
       </c>
     </row>
     <row r="24" ht="15.75" spans="1:3">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="47" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="13" t="s">
@@ -2407,20 +2510,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="29.6666666666667" style="27" customWidth="1"/>
-    <col min="2" max="2" width="19.2222222222222" style="27" customWidth="1"/>
-    <col min="3" max="3" width="50.6666666666667" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.88888888888889" style="27"/>
+    <col min="1" max="1" width="29.6666666666667" style="31" customWidth="1"/>
+    <col min="2" max="2" width="19.2222222222222" style="31" customWidth="1"/>
+    <col min="3" max="3" width="50.6666666666667" style="31" customWidth="1"/>
+    <col min="4" max="16384" width="8.88888888888889" style="31"/>
   </cols>
   <sheetData>
     <row r="1" s="30" customFormat="1" ht="18" spans="1:4">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="30" t="s">
@@ -2428,11 +2531,11 @@
       </c>
     </row>
     <row r="2" ht="18" spans="1:3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="13" t="s">
@@ -2455,41 +2558,41 @@
       <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="27" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="31" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" ht="45" spans="1:3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="34" t="s">
         <v>45</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="34" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" ht="30" spans="1:3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="34" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="34" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" ht="30" spans="1:3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="34" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -2500,18 +2603,18 @@
       </c>
     </row>
     <row r="9" ht="45" spans="1:3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="34" t="s">
         <v>51</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="34" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="34" t="s">
         <v>53</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -2522,7 +2625,7 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="34" t="s">
         <v>54</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -2533,7 +2636,7 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="34" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -2544,7 +2647,7 @@
       </c>
     </row>
     <row r="13" ht="30" spans="1:3">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="34" t="s">
         <v>56</v>
       </c>
       <c r="B13" s="13" t="s">
@@ -2555,7 +2658,7 @@
       </c>
     </row>
     <row r="14" ht="30" spans="1:3">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="34" t="s">
         <v>57</v>
       </c>
       <c r="B14" s="13" t="s">
@@ -2565,12 +2668,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" s="27" customFormat="1" ht="18" spans="1:3">
-      <c r="A15" s="32" t="s">
+    <row r="15" s="31" customFormat="1" ht="18" spans="1:3">
+      <c r="A15" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="13" t="s">
@@ -2701,58 +2804,58 @@
       <c r="C27" s="13"/>
     </row>
     <row r="28" ht="18" spans="1:3">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
     </row>
     <row r="29" ht="30" spans="1:3">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="34" t="s">
         <v>81</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="34" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="30" ht="45" spans="1:3">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="34" t="s">
         <v>83</v>
       </c>
       <c r="B30" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="34" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="31" ht="30" spans="1:3">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="34" t="s">
         <v>85</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="34" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="32" ht="30" spans="1:3">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="34" t="s">
         <v>87</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="34" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="33" spans="3:3">
-      <c r="C33" s="27">
+      <c r="C33" s="31">
         <v>87</v>
       </c>
     </row>
@@ -2778,525 +2881,630 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z22"/>
+  <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.6666666666667" customWidth="1"/>
-    <col min="3" max="3" width="19.8888888888889" customWidth="1"/>
-    <col min="4" max="4" width="28.4444444444444" customWidth="1"/>
-    <col min="5" max="5" width="29.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="22.5555555555556" customWidth="1"/>
-    <col min="7" max="7" width="9.22222222222222" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="1" max="1" width="18.4444444444444" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.6666666666667" style="8" customWidth="1"/>
+    <col min="3" max="3" width="19.8888888888889" style="8" customWidth="1"/>
+    <col min="4" max="4" width="28.4444444444444" style="8" customWidth="1"/>
+    <col min="5" max="5" width="29.6666666666667" style="8" customWidth="1"/>
+    <col min="6" max="6" width="22.5555555555556" style="8" customWidth="1"/>
+    <col min="7" max="7" width="9.22222222222222" style="8" customWidth="1"/>
+    <col min="8" max="8" width="14" style="8" customWidth="1"/>
+    <col min="9" max="9" width="8.88888888888889" style="8"/>
+    <col min="10" max="16384" width="8.88888888888889" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A1" s="8" t="s">
+    <row r="1" customFormat="1" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A1" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-    </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A2" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-    </row>
-    <row r="3" ht="45" spans="1:8">
-      <c r="A3" s="11">
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+    </row>
+    <row r="2" customFormat="1" ht="45" spans="1:9">
+      <c r="A2" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" s="15">
         <v>1</v>
       </c>
+    </row>
+    <row r="3" customFormat="1" ht="60" spans="1:9">
+      <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>100</v>
+      <c r="C3" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>8</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="H3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" ht="60" spans="1:8">
-      <c r="A4" s="11">
+      <c r="H3" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" s="15">
         <v>2</v>
       </c>
+    </row>
+    <row r="4" customFormat="1" ht="75" spans="1:9">
+      <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>8</v>
+        <v>108</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="H4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" ht="60" spans="1:8">
-      <c r="A5" s="11">
+      <c r="H4" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I4" s="15">
         <v>3</v>
       </c>
+    </row>
+    <row r="5" customFormat="1" ht="75.75" spans="1:9">
+      <c r="A5" s="11"/>
       <c r="B5" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="G5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="H5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" ht="75.75" spans="1:8">
-      <c r="A6" s="11">
+      <c r="H5" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I5" s="15">
         <v>4</v>
       </c>
+    </row>
+    <row r="6" customFormat="1" ht="75" spans="1:9">
+      <c r="A6" s="11"/>
       <c r="B6" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>113</v>
+        <v>23</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="H6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" ht="90" spans="1:8">
-      <c r="A7" s="11">
+      <c r="H6" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" s="15">
         <v>5</v>
       </c>
+    </row>
+    <row r="7" customFormat="1" ht="60" spans="1:9">
+      <c r="A7" s="11"/>
       <c r="B7" s="12" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>23</v>
+        <v>120</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="H7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" ht="45" spans="1:8">
-      <c r="A8" s="11">
+        <v>121</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7" s="15">
         <v>6</v>
       </c>
+    </row>
+    <row r="8" customFormat="1" ht="45.75" spans="1:9">
+      <c r="A8" s="11"/>
       <c r="B8" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I8" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="1" ht="60" spans="1:9">
+      <c r="A9" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="H8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" spans="1:7">
-      <c r="A9" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" ht="60" spans="1:8">
-      <c r="A10" s="11">
-        <v>7</v>
-      </c>
+      <c r="C9" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="1" ht="60" spans="1:9">
+      <c r="A10" s="18"/>
       <c r="B10" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>125</v>
+        <v>118</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>132</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" ht="60" spans="1:8">
-      <c r="A11" s="11">
-        <v>8</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I10" s="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="1" ht="60" spans="1:9">
+      <c r="A11" s="18"/>
       <c r="B11" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C11" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="G11" s="19"/>
-      <c r="H11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" s="7" customFormat="1" ht="60" spans="1:8">
-      <c r="A12" s="21">
-        <v>9</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="G12" s="25"/>
-      <c r="H12" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" ht="60" spans="1:8">
-      <c r="A13" s="11">
+      <c r="E11" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I11" s="15">
         <v>10</v>
       </c>
+    </row>
+    <row r="12" customFormat="1" ht="60" spans="1:9">
+      <c r="A12" s="18"/>
+      <c r="B12" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I12" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="1" ht="105" spans="1:9">
+      <c r="A13" s="18"/>
       <c r="B13" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>135</v>
+        <v>118</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>143</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="G13" s="26"/>
-      <c r="H13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" ht="30" spans="1:6">
-      <c r="A14" s="11">
+        <v>146</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="1" ht="45" spans="1:9">
+      <c r="A14" s="18"/>
+      <c r="B14" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" s="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="1" ht="105.75" spans="1:9">
+      <c r="A15" s="21"/>
+      <c r="B15" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I15" s="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="1" ht="105.75" spans="1:9">
+      <c r="A16" s="21"/>
+      <c r="B16" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I16" s="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" ht="75.75" spans="1:9">
+      <c r="A17" s="22">
+        <v>18</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I17" s="15">
         <v>15</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" ht="45" spans="1:8">
-      <c r="A15" s="11">
+    </row>
+    <row r="18" customFormat="1" ht="60" spans="1:9">
+      <c r="A18" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15">
         <v>16</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="H15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" ht="240" spans="1:8">
-      <c r="A16" s="11">
+    </row>
+    <row r="19" customFormat="1" ht="105" spans="1:9">
+      <c r="A19" s="24"/>
+      <c r="B19" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" customFormat="1" ht="47.25" spans="1:9">
+      <c r="A20" s="25"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" customFormat="1" ht="90" spans="1:9">
+      <c r="A21" s="25"/>
+      <c r="B21" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15">
         <v>17</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="H16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" ht="75" spans="1:8">
-      <c r="A17" s="11">
+    </row>
+    <row r="22" customFormat="1" ht="135" spans="1:9">
+      <c r="A22" s="25"/>
+      <c r="B22" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15">
         <v>18</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="H17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" ht="105" spans="1:6">
-      <c r="A18" s="11">
+    </row>
+    <row r="23" customFormat="1" ht="30" spans="1:9">
+      <c r="A23" s="25"/>
+      <c r="B23" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15">
         <v>19</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" ht="90" spans="3:6">
-      <c r="C19" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="F19" s="27" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" ht="135" spans="3:6">
-      <c r="C20" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="21" ht="30" spans="3:6">
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="F21" s="27"/>
-    </row>
-    <row r="22" ht="47.25" spans="2:6">
-      <c r="B22" t="s">
-        <v>163</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="F22" s="29" t="s">
-        <v>166</v>
-      </c>
+    </row>
+    <row r="24" customFormat="1" ht="15.75" spans="1:9">
+      <c r="A24" s="25"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A16"/>
   </mergeCells>
   <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="Référence"/>
     <hyperlink ref="G3" r:id="rId1" display="Référence"/>
     <hyperlink ref="G4" r:id="rId1" display="Référence"/>
     <hyperlink ref="G5" r:id="rId1" display="Référence"/>
     <hyperlink ref="G6" r:id="rId1" display="Référence"/>
-    <hyperlink ref="G7" r:id="rId1" display="Référence"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3319,132 +3527,132 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="3" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="2" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="1:2">
       <c r="A13" s="4" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="5" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="3" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="6" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="6" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="3" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>